<commit_message>
Quantitativos e Quantitativos em txt
</commit_message>
<xml_diff>
--- a/DB/resultados_qualitativos.xlsx
+++ b/DB/resultados_qualitativos.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{1.0: 3006, 2.0: 2994}</t>
+          <t>{2.0: 3013, 1.0: 2987}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{1.0: 50.1, 2.0: 49.9}</t>
+          <t>{2.0: 50.22, 1.0: 49.78}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,17 +490,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{2.0: 3068, 1.0: 2932}</t>
+          <t>{1.0: 3012, 2.0: 2988}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{2.0: 51.13, 1.0: 48.87}</t>
+          <t>{1.0: 50.2, 2.0: 49.8}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,17 +517,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{2.0: 3039, 1.0: 2961}</t>
+          <t>{1.0: 3034, 2.0: 2966}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{2.0: 50.65, 1.0: 49.35}</t>
+          <t>{1.0: 50.57, 2.0: 49.43}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,12 +544,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{1.0: 2048, 2.0: 1992, 3.0: 1960}</t>
+          <t>{1.0: 2011, 2.0: 1998, 3.0: 1991}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{1.0: 34.13, 2.0: 33.2, 3.0: 32.67}</t>
+          <t>{1.0: 33.52, 2.0: 33.3, 3.0: 33.18}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -571,17 +571,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{1.0: 3005, 2.0: 2995}</t>
+          <t>{2.0: 3003, 1.0: 2997}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{1.0: 50.08, 2.0: 49.92}</t>
+          <t>{2.0: 50.05, 1.0: 49.95}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,17 +598,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{1.0: 2076, 3.0: 1990, 2.0: 1934}</t>
+          <t>{2.0: 2038, 1.0: 2010, 3.0: 1952}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{1.0: 34.6, 3.0: 33.17, 2.0: 32.23}</t>
+          <t>{2.0: 33.97, 1.0: 33.5, 3.0: 32.53}</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -625,17 +625,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{1.0: 3000, 2.0: 3000}</t>
+          <t>{2.0: 3063, 1.0: 2937}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{1.0: 50.0, 2.0: 50.0}</t>
+          <t>{2.0: 51.05, 1.0: 48.95}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -652,17 +652,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{1.0: 3022, 2.0: 2978}</t>
+          <t>{2.0: 3029, 1.0: 2971}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{1.0: 50.37, 2.0: 49.63}</t>
+          <t>{2.0: 50.48, 1.0: 49.52}</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -679,17 +679,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{2.0: 3031, 1.0: 2969}</t>
+          <t>{1.0: 3006, 2.0: 2994}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{2.0: 50.52, 1.0: 49.48}</t>
+          <t>{1.0: 50.1, 2.0: 49.9}</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -706,17 +706,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{1.0: 3014, 2.0: 2986}</t>
+          <t>{2.0: 3098, 1.0: 2902}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{1.0: 50.23, 2.0: 49.77}</t>
+          <t>{2.0: 51.63, 1.0: 48.37}</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -733,12 +733,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{1.0: 3051, 2.0: 2949}</t>
+          <t>{1.0: 3084, 2.0: 2916}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{1.0: 50.85, 2.0: 49.15}</t>
+          <t>{1.0: 51.4, 2.0: 48.6}</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -760,17 +760,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{2.0: 3038, 1.0: 2962}</t>
+          <t>{1.0: 3006, 2.0: 2994}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{2.0: 50.63, 1.0: 49.37}</t>
+          <t>{1.0: 50.1, 2.0: 49.9}</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -787,17 +787,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{1.0: 3009, 2.0: 2991}</t>
+          <t>{2.0: 3045, 1.0: 2955}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{1.0: 50.15, 2.0: 49.85}</t>
+          <t>{2.0: 50.75, 1.0: 49.25}</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -814,12 +814,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{2.0: 3008, 1.0: 2992}</t>
+          <t>{2.0: 3009, 1.0: 2991}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{2.0: 50.13, 1.0: 49.87}</t>
+          <t>{2.0: 50.15, 1.0: 49.85}</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -841,17 +841,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{1.0: 3034, 2.0: 2966}</t>
+          <t>{2.0: 3035, 1.0: 2965}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{1.0: 50.57, 2.0: 49.43}</t>
+          <t>{2.0: 50.58, 1.0: 49.42}</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -868,12 +868,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{2.0: 3003, 1.0: 2997}</t>
+          <t>{2.0: 3056, 1.0: 2944}</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{2.0: 50.05, 1.0: 49.95}</t>
+          <t>{2.0: 50.93, 1.0: 49.07}</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -895,17 +895,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{1.0: 3016, 2.0: 2984}</t>
+          <t>{2.0: 3070, 1.0: 2930}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{1.0: 50.27, 2.0: 49.73}</t>
+          <t>{2.0: 51.17, 1.0: 48.83}</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -922,12 +922,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{2.0: 3009, 1.0: 2991}</t>
+          <t>{2.0: 3070, 1.0: 2930}</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{2.0: 50.15, 1.0: 49.85}</t>
+          <t>{2.0: 51.17, 1.0: 48.83}</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -949,17 +949,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{2.0: 2019, 3.0: 2004, 1.0: 1977}</t>
+          <t>{3.0: 2022, 1.0: 1989, 2.0: 1989}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{2.0: 33.65, 3.0: 33.4, 1.0: 32.95}</t>
+          <t>{3.0: 33.7, 1.0: 33.15, 2.0: 33.15}</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -976,12 +976,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{1.0: 2014, 3.0: 1999, 2.0: 1987}</t>
+          <t>{1.0: 2021, 3.0: 2007, 2.0: 1972}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{1.0: 33.57, 3.0: 33.32, 2.0: 33.12}</t>
+          <t>{1.0: 33.68, 3.0: 33.45, 2.0: 32.87}</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
Add renda familiar em valor discreto
</commit_message>
<xml_diff>
--- a/DB/resultados_qualitativos.xlsx
+++ b/DB/resultados_qualitativos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{2.0: 122, 1.0: 95}</t>
+          <t>{2.0: 118, 1.0: 99}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{2.0: 56.22, 1.0: 43.78}</t>
+          <t>{2.0: 54.38, 1.0: 45.62}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,44 +485,44 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Q5</t>
+          <t>Q4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{2.0: 114, 1.0: 103}</t>
+          <t>{1.0: 54, 2.0: 47, 5.0: 41, 4.0: 40, 3.0: 35}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{2.0: 52.53, 1.0: 47.47}</t>
+          <t>{1.0: 24.88, 2.0: 21.66, 5.0: 18.89, 4.0: 18.43, 3.0: 16.13}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.31</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Q6</t>
+          <t>Q5</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{2.0: 115, 1.0: 102}</t>
+          <t>{2.0: 112, 1.0: 105}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{2.0: 53.0, 1.0: 47.0}</t>
+          <t>{2.0: 51.61, 1.0: 48.39}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -539,130 +539,130 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Q8</t>
+          <t>Q6</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{3.0: 83, 1.0: 73, 2.0: 61}</t>
+          <t>{2.0: 114, 1.0: 103}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{3.0: 38.25, 1.0: 33.64, 2.0: 28.11}</t>
+          <t>{2.0: 52.53, 1.0: 47.47}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.57</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q8</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{2.0: 121, 1.0: 96}</t>
+          <t>{3.0: 78, 2.0: 71, 1.0: 68}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{2.0: 55.76, 1.0: 44.24}</t>
+          <t>{3.0: 35.94, 2.0: 32.72, 1.0: 31.34}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>1.58</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Q12</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{3.0: 73, 2.0: 72, 1.0: 72}</t>
+          <t>{2.0: 120, 1.0: 97}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{3.0: 33.64, 2.0: 33.18, 1.0: 33.18}</t>
+          <t>{2.0: 55.3, 1.0: 44.7}</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>0.99</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Q14</t>
+          <t>Q12</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{1.0: 115, 2.0: 102}</t>
+          <t>{2.0: 84, 1.0: 70, 3.0: 63}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{1.0: 53.0, 2.0: 47.0}</t>
+          <t>{2.0: 38.71, 1.0: 32.26, 3.0: 29.03}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.57</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Q15</t>
+          <t>Q14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{1.0: 111, 2.0: 106}</t>
+          <t>{2.0: 115, 1.0: 102}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{1.0: 51.15, 2.0: 48.85}</t>
+          <t>{2.0: 53.0, 1.0: 47.0}</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -674,17 +674,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Q16</t>
+          <t>Q15</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{1.0: 111, 2.0: 106}</t>
+          <t>{1.0: 123, 2.0: 94}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{1.0: 51.15, 2.0: 48.85}</t>
+          <t>{1.0: 56.68, 2.0: 43.32}</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -694,29 +694,29 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.99</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Q17</t>
+          <t>Q16</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{2.0: 115, 1.0: 102}</t>
+          <t>{1.0: 114, 2.0: 103}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{2.0: 53.0, 1.0: 47.0}</t>
+          <t>{1.0: 52.53, 2.0: 47.47}</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -728,17 +728,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Q18</t>
+          <t>Q17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{1.0: 121, 2.0: 96}</t>
+          <t>{1.0: 112, 2.0: 105}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{1.0: 55.76, 2.0: 44.24}</t>
+          <t>{1.0: 51.61, 2.0: 48.39}</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -748,24 +748,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Q19</t>
+          <t>Q18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{1.0: 112, 2.0: 105}</t>
+          <t>{1.0: 118, 2.0: 99}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{1.0: 51.61, 2.0: 48.39}</t>
+          <t>{1.0: 54.38, 2.0: 45.62}</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -775,29 +775,29 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.99</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Q20</t>
+          <t>Q19</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{1.0: 110, 2.0: 107}</t>
+          <t>{2.0: 116, 1.0: 101}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{1.0: 50.69, 2.0: 49.31}</t>
+          <t>{2.0: 53.46, 1.0: 46.54}</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -809,17 +809,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Q21</t>
+          <t>Q20</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{2.0: 113, 1.0: 104}</t>
+          <t>{2.0: 125, 1.0: 92}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{2.0: 52.07, 1.0: 47.93}</t>
+          <t>{2.0: 57.6, 1.0: 42.4}</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -829,29 +829,29 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.98</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Q22</t>
+          <t>Q21</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{2.0: 122, 1.0: 95}</t>
+          <t>{1.0: 118, 2.0: 99}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{2.0: 56.22, 1.0: 43.78}</t>
+          <t>{1.0: 54.38, 2.0: 45.62}</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -863,22 +863,22 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Q23</t>
+          <t>Q22</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{1.0: 114, 2.0: 103}</t>
+          <t>{2.0: 115, 1.0: 102}</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{1.0: 52.53, 2.0: 47.47}</t>
+          <t>{2.0: 53.0, 1.0: 47.0}</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -890,17 +890,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Q24</t>
+          <t>Q23</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{2.0: 118, 1.0: 99}</t>
+          <t>{2.0: 115, 1.0: 102}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{2.0: 54.38, 1.0: 45.62}</t>
+          <t>{2.0: 53.0, 1.0: 47.0}</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -910,29 +910,29 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Q25</t>
+          <t>Q24</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{1.0: 116, 2.0: 101}</t>
+          <t>{2.0: 112, 1.0: 105}</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{1.0: 53.46, 2.0: 46.54}</t>
+          <t>{2.0: 51.61, 1.0: 48.39}</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -944,52 +944,79 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Q26</t>
+          <t>Q25</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{1.0: 78, 3.0: 74, 2.0: 65}</t>
+          <t>{2.0: 114, 1.0: 103}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{1.0: 35.94, 3.0: 34.1, 2.0: 29.95}</t>
+          <t>{2.0: 52.53, 1.0: 47.47}</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
+          <t>Q26</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>{3.0: 74, 2.0: 72, 1.0: 71}</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{3.0: 34.1, 2.0: 33.18, 1.0: 32.72}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
           <t>Q27</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>{1.0: 76, 3.0: 72, 2.0: 69}</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>{1.0: 35.02, 3.0: 33.18, 2.0: 31.8}</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>{1.0: 79, 2.0: 75, 3.0: 63}</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{1.0: 36.41, 2.0: 34.56, 3.0: 29.03}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>1.58</t>
         </is>

</xml_diff>